<commit_message>
API AND UI testing framewrk.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/data.xlsx
+++ b/src/test/resources/TestData/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="API_Data" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="72">
   <si>
     <t>TCName</t>
   </si>
@@ -73,13 +73,205 @@
   </si>
   <si>
     <t>vtiger CRM - Commercial Open Source CRM</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <r>
+      <t>api</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2A00FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>/users?page=2</t>
+    </r>
+  </si>
+  <si>
+    <t>StatusLine</t>
+  </si>
+  <si>
+    <t>HTTP/1.1 200 OK</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">TC01_validate Get API List Users page </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Get</t>
+  </si>
+  <si>
+    <r>
+      <t>api</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2A00FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>/users?page=1</t>
+    </r>
+  </si>
+  <si>
+    <t>TC02_validate Get API List Users page 1</t>
+  </si>
+  <si>
+    <t>Validation1</t>
+  </si>
+  <si>
+    <t>Validation2</t>
+  </si>
+  <si>
+    <t>Validation3</t>
+  </si>
+  <si>
+    <t>Validation4</t>
+  </si>
+  <si>
+    <t>Validation5</t>
+  </si>
+  <si>
+    <t>Validation6</t>
+  </si>
+  <si>
+    <t>data[2].first_name==Emma</t>
+  </si>
+  <si>
+    <t>data[0].id==1</t>
+  </si>
+  <si>
+    <t>data[0].email==george.bluth@reqres.in</t>
+  </si>
+  <si>
+    <t>data[0].last_name==Lawson</t>
+  </si>
+  <si>
+    <t>Validation7</t>
+  </si>
+  <si>
+    <t>Validation8</t>
+  </si>
+  <si>
+    <t>Validation9</t>
+  </si>
+  <si>
+    <t>Validation10</t>
+  </si>
+  <si>
+    <t>data[2].email==tobias.funke@reqres.in</t>
+  </si>
+  <si>
+    <t>data[2].first_name==Tobias</t>
+  </si>
+  <si>
+    <t>data[2].last_name==Funke</t>
+  </si>
+  <si>
+    <t>TC03_validate Get API List Users</t>
+  </si>
+  <si>
+    <t>api/users/2</t>
+  </si>
+  <si>
+    <t>data.id==2</t>
+  </si>
+  <si>
+    <t>data.email==janet.weaver@reqres.in</t>
+  </si>
+  <si>
+    <t>data.first_name==Janet</t>
+  </si>
+  <si>
+    <t>TC04_Creat User</t>
+  </si>
+  <si>
+    <t>api/users</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>Ekta</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Job</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>CreateUser.json</t>
+  </si>
+  <si>
+    <t>name==Ekta</t>
+  </si>
+  <si>
+    <t>job==Manager</t>
+  </si>
+  <si>
+    <t>HTTP/1.1 301 Moved Permanently</t>
+  </si>
+  <si>
+    <t>TC05_Update User</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>job==CEO</t>
+  </si>
+  <si>
+    <t>TC06_UpdatePatch User</t>
+  </si>
+  <si>
+    <t>Prasad</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>name==Mishra</t>
+  </si>
+  <si>
+    <t>name==Prasad</t>
+  </si>
+  <si>
+    <t>job==MD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +282,46 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF7D7D7D"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -119,18 +351,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -209,6 +464,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -243,6 +499,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -418,20 +675,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.33203125" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,7 +711,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -468,7 +725,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -479,7 +736,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -490,7 +747,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -501,7 +758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -528,24 +785,270 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" customWidth="1"/>
+    <col min="6" max="6" width="7.77734375" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
+    <col min="9" max="9" width="28.88671875" customWidth="1"/>
+    <col min="10" max="10" width="21.21875" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" customWidth="1"/>
+    <col min="14" max="14" width="9.88671875" customWidth="1"/>
+    <col min="15" max="15" width="10" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>